<commit_message>
Update Bug Report Bosch6April.xlsx
</commit_message>
<xml_diff>
--- a/Bug Report Bosch6April.xlsx
+++ b/Bug Report Bosch6April.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Summery" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="96">
   <si>
     <t>Lead Dev: Vikash Jha/ Ranjeet</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t xml:space="preserve">Date of downloading the report is 16th april.                                                  bhavya-123                                          M5G9FUQZ42                                                       Service.Advisor1                                    Welcome@1234 </t>
+  </si>
+  <si>
+    <t>DealerTaxInvoiceClientUAT</t>
   </si>
 </sst>
 </file>
@@ -493,7 +496,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -566,12 +569,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -687,6 +701,9 @@
     </xf>
     <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -969,15 +986,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:F10"/>
+  <dimension ref="B6:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="25.42578125" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
   </cols>
@@ -1035,22 +1052,39 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="5">
         <v>6</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="5">
+        <v>6</v>
+      </c>
+      <c r="E10" s="6">
+        <v>6</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
         <f>SUM(C9:C9)</f>
         <v>6</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <f>SUM(D9)</f>
         <v>6</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E11" s="2">
         <f>SUM(E9:E9)</f>
         <v>6</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F11" s="3">
         <f>SUM(F9:F9)</f>
         <v>0</v>
       </c>
@@ -1722,7 +1756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>

</xml_diff>